<commit_message>
🙍🐉 Updated with Glitch
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\swgoh\shard-payout-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{46B6645A-7506-4B9A-9B6E-00ADAB4929E5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9B7634D0-4032-4D71-AC92-BDDDD0E8BF8D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <customWorkbookViews>
+    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -249,9 +249,6 @@
     <t>DavraMcRay</t>
   </si>
   <si>
-    <t>Pistolpete</t>
-  </si>
-  <si>
     <t>:flag_white:</t>
   </si>
   <si>
@@ -298,6 +295,9 @@
   </si>
   <si>
     <t>puppy juicer</t>
+  </si>
+  <si>
+    <t>dingo slayer</t>
   </si>
 </sst>
 </file>
@@ -1067,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,13 +1302,13 @@
     <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="52"/>
       <c r="B4" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -1500,13 +1500,13 @@
     <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
       <c r="B7" s="18" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="20"/>
@@ -1632,13 +1632,13 @@
     <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
       <c r="B9" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -2229,7 +2229,7 @@
     <row r="18" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="52"/>
       <c r="B18" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -2565,7 +2565,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -2691,7 +2691,7 @@
     <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="52"/>
       <c r="B25" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -2763,7 +2763,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
@@ -2829,7 +2829,7 @@
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
       <c r="F27" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
@@ -2955,7 +2955,7 @@
     <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="52"/>
       <c r="B29" s="40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
@@ -3087,7 +3087,7 @@
     <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="52"/>
       <c r="B31" s="40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -3419,7 +3419,7 @@
     <row r="36" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="52"/>
       <c r="B36" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -3485,7 +3485,7 @@
     <row r="37" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="52"/>
       <c r="B37" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -3749,7 +3749,7 @@
     <row r="41" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="52"/>
       <c r="B41" s="41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -3815,7 +3815,7 @@
     <row r="42" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="52"/>
       <c r="B42" s="41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -4145,7 +4145,7 @@
     <row r="47" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="52"/>
       <c r="B47" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -4343,7 +4343,7 @@
     <row r="50" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="52"/>
       <c r="B50" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -4481,7 +4481,7 @@
       <c r="D52" s="19"/>
       <c r="E52" s="19"/>
       <c r="F52" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G52" s="20"/>
       <c r="H52" s="20"/>
@@ -4609,11 +4609,11 @@
     <sortCondition ref="B27"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
+      <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
-      <selection sqref="A1:XFD1048576"/>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
🌕🚵 Updated with Glitch
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Desktop\swgoh\shard-payout-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9B7634D0-4032-4D71-AC92-BDDDD0E8BF8D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{41ED1B79-66D6-4107-A779-310D73A09674}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>dingo slayer</t>
+  </si>
+  <si>
+    <t>HBP</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X53"/>
+  <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="V1" s="5">
-        <f>H53</f>
+        <f>H54</f>
         <v>0</v>
       </c>
     </row>
@@ -4541,7 +4544,7 @@
     <row r="53" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="52"/>
       <c r="B53" s="40" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="19"/>
@@ -4550,11 +4553,11 @@
         <v>60</v>
       </c>
       <c r="G53" s="20"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="21">
+      <c r="H53" s="20"/>
+      <c r="I53" s="8">
         <v>0.125</v>
       </c>
-      <c r="J53" s="22"/>
+      <c r="J53" s="10"/>
       <c r="K53" s="14">
         <f>$I53+Sheet2!B$1/24</f>
         <v>0.54166666666666674</v>
@@ -4601,6 +4604,72 @@
       </c>
       <c r="V53" s="16">
         <f>$I53+Sheet2!B$12/24</f>
+        <v>-0.16666666666666669</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="52"/>
+      <c r="B54" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G54" s="20"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="21">
+        <v>0.125</v>
+      </c>
+      <c r="J54" s="22"/>
+      <c r="K54" s="14">
+        <f>$I54+Sheet2!B$1/24</f>
+        <v>0.54166666666666674</v>
+      </c>
+      <c r="L54" s="14">
+        <f>$I54+Sheet2!B$2/24</f>
+        <v>0.5</v>
+      </c>
+      <c r="M54" s="14">
+        <f>$I54+Sheet2!B$3/24</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="N54" s="14">
+        <f>$I54+Sheet2!B$4/24</f>
+        <v>0.25</v>
+      </c>
+      <c r="O54" s="14">
+        <f>$I54+Sheet2!B$5/24</f>
+        <v>0.25</v>
+      </c>
+      <c r="P54" s="14">
+        <f>$I54+Sheet2!B$6/24</f>
+        <v>0.25</v>
+      </c>
+      <c r="Q54" s="14">
+        <f>$I54+Sheet2!B$7/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="R54" s="14">
+        <f>$I54+Sheet2!B$8/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="S54" s="14">
+        <f>$I54+Sheet2!B$9/24</f>
+        <v>-4.1666666666666657E-2</v>
+      </c>
+      <c r="T54" s="14">
+        <f>$I54+Sheet2!B$10/24</f>
+        <v>-8.3333333333333343E-2</v>
+      </c>
+      <c r="U54" s="14">
+        <f>$I54+Sheet2!B$11/24</f>
+        <v>-0.125</v>
+      </c>
+      <c r="V54" s="16">
+        <f>$I54+Sheet2!B$12/24</f>
         <v>-0.16666666666666669</v>
       </c>
     </row>
@@ -4609,30 +4678,30 @@
     <sortCondition ref="B27"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="3">
     <mergeCell ref="A11:A33"/>
-    <mergeCell ref="A34:A53"/>
+    <mergeCell ref="A34:A54"/>
     <mergeCell ref="A2:A10"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L2 K3:V53">
+  <conditionalFormatting sqref="K2:L2 K3:V54">
     <cfRule type="expression" dxfId="2" priority="17">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:V53">
+  <conditionalFormatting sqref="K2:V54">
     <cfRule type="expression" dxfId="1" priority="19">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:V53">
+  <conditionalFormatting sqref="B2:V54">
     <cfRule type="expression" dxfId="0" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>